<commit_message>
feb 14th update, juzgados
</commit_message>
<xml_diff>
--- a/resources/juzgados.xlsx
+++ b/resources/juzgados.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" dateCompatibility="false"/>
+  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
@@ -46,6 +46,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -66,6 +67,7 @@
       <sz val="10"/>
       <name val="Times New Roman"/>
       <family val="1"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -110,7 +112,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -121,6 +123,10 @@
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -140,13 +146,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:BC60"/>
+  <dimension ref="A1:BD62"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A61" activeCellId="0" sqref="A61"/>
+      <selection pane="topLeft" activeCell="G31" activeCellId="0" sqref="G31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -9787,166 +9793,498 @@
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="2"/>
-      <c r="B60" s="1" t="n">
+      <c r="B60" s="3" t="n">
+        <v>5</v>
+      </c>
+      <c r="C60" s="3" t="n">
+        <v>1584</v>
+      </c>
+      <c r="D60" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E60" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="F60" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G60" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="H60" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I60" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="J60" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="K60" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="L60" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="M60" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="N60" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="O60" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="P60" s="3" t="n">
+        <v>6137</v>
+      </c>
+      <c r="Q60" s="3" t="n">
+        <v>7777</v>
+      </c>
+      <c r="R60" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="S60" s="3" t="n">
+        <v>1079</v>
+      </c>
+      <c r="T60" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="U60" s="3" t="n">
+        <v>8047</v>
+      </c>
+      <c r="V60" s="3" t="n">
+        <v>1017</v>
+      </c>
+      <c r="W60" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="X60" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y60" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z60" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA60" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB60" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC60" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD60" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE60" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AF60" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG60" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AH60" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI60" s="3" t="n">
+        <v>1020</v>
+      </c>
+      <c r="AJ60" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK60" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL60" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM60" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN60" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AO60" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AP60" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AQ60" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AR60" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS60" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AT60" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AU60" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AV60" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AW60" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AX60" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AY60" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AZ60" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="BA60" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="BB60" s="3" t="n">
+        <v>6282</v>
+      </c>
+      <c r="BC60" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="BD60" s="3"/>
+    </row>
+    <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A61" s="2"/>
+      <c r="B61" s="3" t="n">
+        <v>6</v>
+      </c>
+      <c r="C61" s="3" t="n">
+        <v>1772</v>
+      </c>
+      <c r="D61" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E61" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="F61" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G61" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="H61" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I61" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="J61" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="K61" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="L61" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="M61" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="N61" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="O61" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="P61" s="3" t="n">
+        <v>6922</v>
+      </c>
+      <c r="Q61" s="3" t="n">
+        <v>8757</v>
+      </c>
+      <c r="R61" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="S61" s="3" t="n">
+        <v>1224</v>
+      </c>
+      <c r="T61" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="U61" s="3" t="n">
+        <v>8982</v>
+      </c>
+      <c r="V61" s="3" t="n">
+        <v>1177</v>
+      </c>
+      <c r="W61" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="X61" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y61" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z61" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA61" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB61" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC61" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD61" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE61" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AF61" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG61" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AH61" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI61" s="3" t="n">
+        <v>1156</v>
+      </c>
+      <c r="AJ61" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK61" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL61" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM61" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN61" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AO61" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AP61" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AQ61" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AR61" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS61" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AT61" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AU61" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AV61" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AW61" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AX61" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AY61" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AZ61" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="BA61" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="BB61" s="3" t="n">
+        <v>6924</v>
+      </c>
+      <c r="BC61" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="BD61" s="3"/>
+    </row>
+    <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A62" s="2"/>
+      <c r="B62" s="1" t="n">
         <v>53</v>
       </c>
-      <c r="C60" s="1" t="n">
+      <c r="C62" s="1" t="n">
         <v>114</v>
       </c>
-      <c r="D60" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="E60" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="F60" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="G60" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="H60" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="I60" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="J60" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="K60" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="L60" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="M60" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="N60" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="O60" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="P60" s="1" t="n">
+      <c r="D62" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="E62" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="F62" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="G62" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="H62" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="I62" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="J62" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="K62" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="L62" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="M62" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="N62" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="O62" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="P62" s="1" t="n">
         <v>460</v>
       </c>
-      <c r="Q60" s="1" t="n">
+      <c r="Q62" s="1" t="n">
         <v>491</v>
       </c>
-      <c r="R60" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="S60" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="T60" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="U60" s="1" t="n">
+      <c r="R62" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="S62" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="T62" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="U62" s="1" t="n">
         <v>653</v>
       </c>
-      <c r="V60" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="W60" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="X60" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="Y60" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="Z60" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="AA60" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="AB60" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="AC60" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="AD60" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="AE60" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="AF60" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="AG60" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="AH60" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="AI60" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="AJ60" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="AK60" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="AL60" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="AM60" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="AN60" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="AO60" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="AP60" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="AQ60" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="AR60" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="AS60" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="AT60" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="AU60" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="AV60" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="AW60" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="AX60" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="AY60" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="AZ60" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="BA60" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="BB60" s="1" t="n">
+      <c r="V62" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="W62" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="X62" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y62" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z62" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA62" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB62" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC62" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD62" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE62" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AF62" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG62" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AH62" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI62" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ62" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK62" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL62" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM62" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN62" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AO62" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AP62" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AQ62" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AR62" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS62" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AT62" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AU62" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AV62" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AW62" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AX62" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AY62" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AZ62" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BA62" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BB62" s="1" t="n">
         <v>584</v>
       </c>
-      <c r="BC60" s="1" t="n">
+      <c r="BC62" s="1" t="n">
         <v>0</v>
       </c>
     </row>

</xml_diff>